<commit_message>
NEW: Ejercicios sobre abstraccion
</commit_message>
<xml_diff>
--- a/material/IntroProg/Notas/Quices.xlsx
+++ b/material/IntroProg/Notas/Quices.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCABDB5A-DB43-4A46-9227-A57BBC20CC7B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE0E1F8-A2C1-4ED2-AF7C-DDF9C42D7CA3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13,12 +13,20 @@
   <definedNames>
     <definedName name="JR_PAGE_ANCHOR_0_1">'report name'!$A$1</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="91">
   <si>
     <t>Introducción a la Programación</t>
   </si>
@@ -125,20 +133,191 @@
     <t>Burgos Avendaño,Carlos Alberto</t>
   </si>
   <si>
-    <t>Pendiente calificar completo</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>Correa, Camilo ( No aparece en lista)</t>
+    <t>Quiz 10 Feb - part1  Generacion E
+Condicionales anidados y enlazados</t>
+  </si>
+  <si>
+    <t>Errores de sintaxis en condicionales
+Los mensajes no explican bien las condiciones por la que no se cumple la generación e
+Los condicionales estan más largo de lo que deberían pero funcionan</t>
+  </si>
+  <si>
+    <t>Grupo</t>
+  </si>
+  <si>
+    <t>Usa elif lo que hace que en algunos casos no se muestren las dos condiciones 
+Usa diferente, no mayor y menor igual</t>
+  </si>
+  <si>
+    <t>Condición lógica
+Elif</t>
+  </si>
+  <si>
+    <t>Condición lógica
+Código  más complejo</t>
+  </si>
+  <si>
+    <t>Puso las condiciones al revés, la condición de entrada está bn par el primer if en el que evalúa las dos, pero luego en vez de poner el siguiente if dentro del else lo puso dentro del if</t>
+  </si>
+  <si>
+    <t>Cómo ubicar los condicionales anidados</t>
+  </si>
+  <si>
+    <t>Solo puso condicional sencillo, no hizo la lógica para que contestara a las dos preguntas</t>
+  </si>
+  <si>
+    <t>Usar condicionales enlazados y anidados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Como ubiacr los condicionales
+Orden de aparición d las variables, </t>
+  </si>
+  <si>
+    <t>Pregunta dentro de if entonces no va a preguntar en todos los casos
+Elif sin if, entones error de sintaxis. Suponiendo que fuera un if, entonces si entraría. 
+Problemas en como pone los condicionales</t>
+  </si>
+  <si>
+    <t>Doble else sin un if</t>
+  </si>
+  <si>
+    <t>Tiene doble else, el mensaje del print no explica bn pq no puede participar.  Tiene más o menos la lógica</t>
+  </si>
+  <si>
+    <t>ya le dije</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>condición de entrada mala, código más complejo de lo necesario</t>
+  </si>
+  <si>
+    <t>Confusión entre if y elif</t>
+  </si>
+  <si>
+    <t>En el caso de que no cumple con los dos requisitos no imprime el mensaje. Tiene un print con una aclaración pero me gustarí más que lo hiciera con un else</t>
+  </si>
+  <si>
+    <t>Muchos elfi</t>
+  </si>
+  <si>
+    <t>Podría hacero de manera más sencilla</t>
+  </si>
+  <si>
+    <t>Varias condiciones separadas
+Me gusta la idea de la variable bandera</t>
+  </si>
+  <si>
+    <t>Muchas condiciones</t>
+  </si>
+  <si>
+    <t>Falla en cso de GE flse y porcenaje &gt; 25</t>
+  </si>
+  <si>
+    <t>Falla cuando acreditada es No y oferta es no por el orden de los elif</t>
+  </si>
+  <si>
+    <t>Orde de los condicionales</t>
+  </si>
+  <si>
+    <t>Usa if en lugar del elf, aunque las condiciones estan bn</t>
+  </si>
+  <si>
+    <t>Falla cuando acreditacion No, y porcentaje SI y viceversa</t>
+  </si>
+  <si>
+    <t>Falla pq digo cuál o cuales condiciones siempre muestra el error por las dos cosas. 
+Me parece que tiene buena logica y puede arreglarlo</t>
+  </si>
+  <si>
+    <t>Orde de los condicionales del elif</t>
+  </si>
+  <si>
+    <t>Falla cuando intitu no y porcentaje tampoco, problemas en el ==
+Creo que tiene buena lógicca</t>
+  </si>
+  <si>
+    <t>Le falta pedir el valor de la oferta academica para saber si cumple con el valor o no.  Puede que tenga la lógica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ejercicio incompleto, solo funciona si acreditada de alta calidad </t>
+  </si>
+  <si>
+    <t>NO encadenó las cosas bn, tiene errores de sintaxis, la solución no hace nada</t>
+  </si>
+  <si>
+    <t>Sintaxis, orden de los condicionales, lógica en general</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>----</t>
+  </si>
+  <si>
+    <t>Solo, no sé que le pasó</t>
+  </si>
+  <si>
+    <t>( No vino a clase)</t>
+  </si>
+  <si>
+    <t>No vino</t>
+  </si>
+  <si>
+    <t>Observación</t>
+  </si>
+  <si>
+    <t>Al ponerlo con alguien que estaba muy perdido, los dos estaban super perdidos.  Entonces no esta funcionando como explicación</t>
+  </si>
+  <si>
+    <t>no se ayudaron</t>
+  </si>
+  <si>
+    <t>decima</t>
+  </si>
+  <si>
+    <t>si se ayudaron</t>
+  </si>
+  <si>
+    <t>si se ayudaronm pero luego de que les dje</t>
+  </si>
+  <si>
+    <t>quedo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">se ayudatom                                 </t>
+  </si>
+  <si>
+    <t>se ayudaron mas o menos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       </t>
+  </si>
+  <si>
+    <t>cada uno miro su codigo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                </t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t>No lo entrego</t>
+  </si>
+  <si>
+    <t>Décima parcial</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,6 +353,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -200,7 +415,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -258,11 +473,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -272,9 +496,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -287,6 +508,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -605,292 +853,940 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="96" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="96" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" customWidth="1"/>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="20.109375" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10" style="3" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" style="3" customWidth="1"/>
+    <col min="4" max="5" width="21.6640625" style="6" customWidth="1"/>
+    <col min="6" max="7" width="21.88671875" style="11" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" style="6" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" style="3"/>
+    <col min="11" max="11" width="18.33203125" style="3" customWidth="1"/>
+    <col min="12" max="59" width="8.88671875" style="3"/>
+    <col min="60" max="60" width="11.109375" style="3" customWidth="1"/>
+    <col min="61" max="72" width="8.88671875" style="3"/>
+    <col min="73" max="73" width="8.6640625" style="3" customWidth="1"/>
+    <col min="74" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="31.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:14" ht="31.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="N2"/>
+    </row>
+    <row r="3" spans="1:14" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="3">
+        <v>5</v>
+      </c>
+      <c r="C3" s="6">
+        <v>5</v>
+      </c>
+      <c r="D3" s="6">
+        <v>4</v>
+      </c>
+      <c r="E3" s="6">
+        <v>5</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" s="6">
+        <v>10</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="7">
+      <c r="B4" s="3">
+        <v>5</v>
+      </c>
+      <c r="C4" s="6">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="6">
+        <v>3</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="6">
+        <v>1</v>
+      </c>
+      <c r="J4" s="3">
+        <v>5</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="7">
+      <c r="B5" s="3">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="6">
+        <v>2</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="6">
+        <v>2</v>
+      </c>
+      <c r="J5" s="3">
+        <v>5</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="3">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6">
+        <v>5</v>
+      </c>
+      <c r="D6" s="6">
+        <v>2</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="6">
+        <v>4</v>
+      </c>
+      <c r="J6" s="3">
+        <v>5</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="7">
+      <c r="B7" s="3">
+        <v>5</v>
+      </c>
+      <c r="C7" s="6">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="6">
+        <v>4</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="H7" s="6">
+        <v>8</v>
+      </c>
+      <c r="J7" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="7">
+      <c r="B8" s="3">
+        <v>5</v>
+      </c>
+      <c r="C8" s="6">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="6">
+        <v>2</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="14">
+        <v>4</v>
+      </c>
+      <c r="J8" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="7">
+      <c r="B9" s="3">
+        <v>5</v>
+      </c>
+      <c r="C9" s="6">
         <v>4.8</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="12">
+        <v>1</v>
+      </c>
+      <c r="E9" s="12"/>
+      <c r="F9" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+      <c r="B10" s="3">
+        <v>5</v>
+      </c>
+      <c r="C10" s="6">
+        <v>5</v>
+      </c>
+      <c r="D10" s="6">
+        <v>4.8</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" s="6">
+        <v>6</v>
+      </c>
+      <c r="J10" s="3">
+        <v>5</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3">
+        <v>5</v>
+      </c>
+      <c r="C11" s="6">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D11" s="6">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="H11" s="6">
+        <v>9</v>
+      </c>
+      <c r="J11" s="3">
+        <v>5</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="C12" s="6">
+        <v>4.8</v>
+      </c>
+      <c r="D12" s="6">
+        <v>4</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" s="6">
+        <v>8</v>
+      </c>
+      <c r="J12" s="3">
+        <v>5</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="31.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="C13" s="6">
+        <v>5</v>
+      </c>
+      <c r="D13" s="6">
+        <v>4.5</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="H13" s="6">
+        <v>12</v>
+      </c>
+      <c r="J13" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="C14" s="6">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="D14" s="6">
+        <v>5</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="J14" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="3">
+        <v>5</v>
+      </c>
+      <c r="C15" s="6">
+        <v>5</v>
+      </c>
+      <c r="D15" s="6">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="H15" s="6">
+        <v>6</v>
+      </c>
+      <c r="I15" s="3">
+        <v>5</v>
+      </c>
+      <c r="J15" s="3">
+        <v>5</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="3">
+        <v>5</v>
+      </c>
+      <c r="C16" s="6">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="D16" s="6">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16" s="6">
+        <v>7</v>
+      </c>
+      <c r="J16" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="3">
+        <v>3</v>
+      </c>
+      <c r="C17" s="6">
+        <v>4.3</v>
+      </c>
+      <c r="D17" s="6">
+        <v>3</v>
+      </c>
+      <c r="F17" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="7">
-        <v>4.5999999999999996</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="G17" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H17" s="6">
+        <v>1</v>
+      </c>
+      <c r="J17" s="3">
+        <v>5</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="C18" s="6">
+        <v>3.7</v>
+      </c>
+      <c r="D18" s="6">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="H18" s="6">
+        <v>6</v>
+      </c>
+      <c r="J18" s="3">
+        <v>5</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="3">
+        <v>5</v>
+      </c>
+      <c r="C19" s="6">
+        <v>4.8</v>
+      </c>
+      <c r="D19" s="6">
+        <v>2</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" s="12">
+        <v>4</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="J19" s="3">
+        <v>5</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="3">
+        <v>5</v>
+      </c>
+      <c r="C20" s="6">
+        <v>5</v>
+      </c>
+      <c r="D20" s="6">
+        <v>5</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="J20" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="3">
+        <v>4</v>
+      </c>
+      <c r="C21" s="6">
+        <v>3.4</v>
+      </c>
+      <c r="D21" s="6">
+        <v>3.75</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="H21" s="6">
+        <v>3</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="J21" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="C22" s="6">
+        <v>3.3</v>
+      </c>
+      <c r="D22" s="6">
+        <v>4.5</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="H22" s="6">
         <v>9</v>
       </c>
-      <c r="C12" s="7">
-        <v>4.5999999999999996</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="J22" s="3">
+        <v>5</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="C23" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="D23" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H23" s="6">
+        <v>3</v>
+      </c>
+      <c r="J23" s="3">
+        <v>5</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="3">
+        <v>5</v>
+      </c>
+      <c r="C24" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="D24" s="6">
+        <v>5</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="J24" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="3">
+        <v>5</v>
+      </c>
+      <c r="C25" s="6">
+        <v>5</v>
+      </c>
+      <c r="D25" s="6">
+        <v>3</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="H25" s="6">
+        <v>2</v>
+      </c>
+      <c r="J25" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="3">
+        <v>5</v>
+      </c>
+      <c r="C26" s="6">
+        <v>4.8</v>
+      </c>
+      <c r="D26" s="6">
+        <v>4.5</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="H26" s="6">
+        <v>8</v>
+      </c>
+      <c r="J26" s="3">
+        <v>5</v>
+      </c>
+      <c r="K26" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="3">
+        <v>5</v>
+      </c>
+      <c r="C27" s="6">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="D27" s="6">
+        <v>3</v>
+      </c>
+      <c r="E27" s="6">
+        <v>5</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="H27" s="6">
         <v>10</v>
       </c>
-      <c r="C13" s="7">
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="7" t="s">
+      <c r="J27" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="3">
+        <v>5</v>
+      </c>
+      <c r="C28" s="7" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+      <c r="D28" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K28" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L28" s="6"/>
+    </row>
+    <row r="29" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="3">
+        <v>3</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="C30" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="C31" s="6">
+        <v>3</v>
+      </c>
+      <c r="D31" s="6">
+        <v>4.5</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="H31" s="6">
         <v>12</v>
       </c>
-      <c r="C15" s="7">
-        <v>4.8499999999999996</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="7">
+      <c r="J31" s="3">
+        <v>5</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="C32" s="6">
+        <v>5</v>
+      </c>
+      <c r="D32" s="6">
+        <v>5</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="J32" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="3">
+        <v>5</v>
+      </c>
+      <c r="C33" s="6">
+        <v>5</v>
+      </c>
+      <c r="D33" s="6">
         <v>4.9000000000000004</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="7">
-        <v>4.3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="7">
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="7">
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="7">
-        <v>3.4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="7">
-        <v>3.3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="7">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="7">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="7">
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" s="7">
-        <v>4.8499999999999996</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31" s="7">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C34" s="7">
-        <v>5</v>
+      <c r="F33" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="H33" s="6">
+        <v>7</v>
+      </c>
+      <c r="J33" s="3">
+        <v>5</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D2:F2"/>
+  </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>

</xml_diff>